<commit_message>
Updates to schedule, master list.
</commit_message>
<xml_diff>
--- a/EdSight_Datasets_Summary.xlsx
+++ b/EdSight_Datasets_Summary.xlsx
@@ -20,36 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">From EdSight (found here: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/CT-Data-Collaborative/edsight-data/tree/master/data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+  <si>
+    <t xml:space="preserve">Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From EdSight (found here: https://github.com/CT-Data-Collaborative/edsight-data/tree/master/data)</t>
   </si>
   <si>
     <t xml:space="preserve">Dataset name</t>
@@ -64,6 +43,9 @@
     <t xml:space="preserve">Complete</t>
   </si>
   <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">annual_expenditures</t>
   </si>
   <si>
@@ -95,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Chronic-Absenteeism-by-All-Students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add CT level data</t>
   </si>
   <si>
     <t xml:space="preserve">bullying_district</t>
@@ -352,13 +337,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -406,17 +391,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -456,549 +457,681 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C4:N63"/>
+  <dimension ref="C3:N63"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.6275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.76530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.1122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.8826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="4" s="1" customFormat="true" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="2" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" s="3" customFormat="true" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
+      <c r="C6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F6" s="8" t="n">
         <v>42809</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="8" t="n">
         <v>42811</v>
       </c>
+      <c r="H6" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="I6" s="8" t="n">
+        <v>42821</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="F7" s="8" t="n">
         <v>42809</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="8" t="n">
         <v>42811</v>
       </c>
+      <c r="H7" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="I7" s="8" t="n">
+        <v>42821</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="F8" s="8" t="n">
         <v>42809</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="8" t="n">
         <v>42811</v>
       </c>
+      <c r="H8" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="I8" s="8" t="n">
+        <v>42821</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="n">
         <v>42809</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="8" t="n">
         <v>42811</v>
       </c>
+      <c r="H9" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="I9" s="8" t="n">
+        <v>42821</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="F10" s="8" t="n">
         <v>42809</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="8" t="n">
         <v>42811</v>
       </c>
+      <c r="H10" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="I10" s="8" t="n">
+        <v>42821</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="F11" s="8" t="n">
         <v>42809</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="8" t="n">
         <v>42811</v>
       </c>
+      <c r="H11" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="I11" s="8" t="n">
+        <v>42821</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="F12" s="8" t="n">
         <v>42809</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="8" t="n">
         <v>42811</v>
       </c>
+      <c r="H12" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="I12" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="4" t="n">
+      <c r="C13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8" t="n">
         <v>42809</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="8" t="n">
         <v>42809</v>
       </c>
+      <c r="H13" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="I13" s="8" t="n">
+        <v>42821</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>19</v>
+      <c r="C14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="F14" s="8" t="n">
+        <v>42815</v>
+      </c>
+      <c r="G14" s="8" t="n">
+        <v>42817</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="6"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="F15" s="8" t="n">
+        <v>42815</v>
+      </c>
+      <c r="G15" s="8" t="n">
+        <v>42817</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="F16" s="8" t="n">
+        <v>42815</v>
+      </c>
+      <c r="G16" s="8" t="n">
+        <v>42817</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="6"/>
-      <c r="D17" s="3"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="F17" s="8" t="n">
+        <v>42815</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <v>42817</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="6"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="F18" s="8" t="n">
+        <v>42815</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <v>42817</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="F19" s="8" t="n">
+        <v>42815</v>
+      </c>
+      <c r="G19" s="8" t="n">
+        <v>42817</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="6"/>
-      <c r="D20" s="3"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="F20" s="8" t="n">
+        <v>42815</v>
+      </c>
+      <c r="G20" s="8" t="n">
+        <v>42817</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="6"/>
-      <c r="D21" s="3"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="F21" s="8" t="n">
+        <v>42815</v>
+      </c>
+      <c r="G21" s="8" t="n">
+        <v>42817</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>29</v>
+      <c r="C22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="N26" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="N26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
       <c r="E27" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N27" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="N27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N28" s="7"/>
+      <c r="C28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N29" s="7"/>
+      <c r="C29" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>41</v>
+      <c r="C30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N30" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="N30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
       <c r="E31" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="N31" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="N31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
       <c r="E32" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="N32" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="N32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
       <c r="E33" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
       <c r="E34" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
       <c r="E35" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>49</v>
+      <c r="C36" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
       <c r="E37" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
       <c r="E38" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
       <c r="E39" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
       <c r="E40" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
       <c r="E41" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
       <c r="E42" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C43" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>58</v>
+      <c r="C43" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="3"/>
-      <c r="D44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="10"/>
       <c r="E44" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="3"/>
-      <c r="D45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="10"/>
       <c r="E45" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="3"/>
-      <c r="D46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="10"/>
       <c r="E46" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="3"/>
-      <c r="D47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="10"/>
       <c r="E47" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="3"/>
-      <c r="D48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="10"/>
       <c r="E48" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="3"/>
-      <c r="D49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="10"/>
       <c r="E49" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>67</v>
+      <c r="C50" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>69</v>
+      <c r="C51" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>71</v>
+      <c r="C52" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>73</v>
+      <c r="C53" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>75</v>
+      <c r="C54" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>77</v>
+      <c r="C55" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>79</v>
+      <c r="C56" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>81</v>
+      <c r="C57" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
       <c r="E58" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
       <c r="E59" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
       <c r="E60" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
       <c r="E61" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
       <c r="E62" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>89</v>
+      <c r="C63" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="C6:C12"/>
     <mergeCell ref="D6:D12"/>
     <mergeCell ref="C14:C21"/>
@@ -1015,7 +1148,7 @@
     <mergeCell ref="D57:D62"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="https://github.com/CT-Data-Collaborative/edsight-data/tree/master/data"/>
+    <hyperlink ref="C4" r:id="rId1" display="From EdSight (found here: https://github.com/CT-Data-Collaborative/edsight-data/tree/master/data)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>